<commit_message>
Correções da aula 1 - Finalizada
</commit_message>
<xml_diff>
--- a/Frequencia/MAF105_T1.xlsx
+++ b/Frequencia/MAF105_T1.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="117">
   <si>
     <t>Nome do Aluno</t>
   </si>
@@ -850,9 +850,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E8" sqref="E8"/>
+      <selection pane="topRight" activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
@@ -1040,8 +1040,12 @@
       <c r="C2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
+      <c r="D2" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
       <c r="H2" s="9"/>
@@ -1078,7 +1082,7 @@
       <c r="AM2" s="9"/>
       <c r="AN2" s="9">
         <f>2*COUNTIF(D2:AM2,"="&amp;$AQ$2)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AO2" s="9">
         <f>2*COUNTIF(D2:AM2,"="&amp;$AR$2)</f>
@@ -1101,8 +1105,12 @@
       <c r="C3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
+      <c r="D3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>10</v>
+      </c>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
@@ -1143,7 +1151,7 @@
       </c>
       <c r="AO3" s="9">
         <f t="shared" ref="AO3:AO52" si="2">2*COUNTIF(D3:AM3,"="&amp;$AR$2)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:44" x14ac:dyDescent="0.2">
@@ -1156,8 +1164,12 @@
       <c r="C4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
+      <c r="D4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
@@ -1194,11 +1206,11 @@
       <c r="AM4" s="9"/>
       <c r="AN4" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO4" s="9">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:44" x14ac:dyDescent="0.2">
@@ -1211,8 +1223,12 @@
       <c r="C5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
+      <c r="D5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
@@ -1249,7 +1265,7 @@
       <c r="AM5" s="9"/>
       <c r="AN5" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AO5" s="9">
         <f t="shared" si="2"/>
@@ -1266,8 +1282,12 @@
       <c r="C6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
+      <c r="D6" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
@@ -1304,7 +1324,7 @@
       <c r="AM6" s="9"/>
       <c r="AN6" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AO6" s="9">
         <f t="shared" si="2"/>
@@ -1321,8 +1341,12 @@
       <c r="C7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
+      <c r="D7" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
@@ -1359,7 +1383,7 @@
       <c r="AM7" s="9"/>
       <c r="AN7" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AO7" s="9">
         <f t="shared" si="2"/>
@@ -1435,8 +1459,12 @@
       <c r="C9" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
+      <c r="D9" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
@@ -1473,7 +1501,7 @@
       <c r="AM9" s="9"/>
       <c r="AN9" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AO9" s="9">
         <f t="shared" si="2"/>
@@ -1490,8 +1518,12 @@
       <c r="C10" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
+      <c r="D10" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>10</v>
+      </c>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
@@ -1528,11 +1560,11 @@
       <c r="AM10" s="9"/>
       <c r="AN10" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO10" s="9">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:44" x14ac:dyDescent="0.2">
@@ -1545,8 +1577,12 @@
       <c r="C11" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
+      <c r="D11" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
@@ -1583,7 +1619,7 @@
       <c r="AM11" s="9"/>
       <c r="AN11" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AO11" s="9">
         <f t="shared" si="2"/>
@@ -1600,8 +1636,12 @@
       <c r="C12" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
+      <c r="D12" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>10</v>
+      </c>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
@@ -1638,11 +1678,11 @@
       <c r="AM12" s="9"/>
       <c r="AN12" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO12" s="9">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:44" x14ac:dyDescent="0.2">
@@ -1655,8 +1695,12 @@
       <c r="C13" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
+      <c r="D13" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
@@ -1693,7 +1737,7 @@
       <c r="AM13" s="9"/>
       <c r="AN13" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AO13" s="9">
         <f t="shared" si="2"/>
@@ -1710,8 +1754,12 @@
       <c r="C14" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
+      <c r="D14" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
@@ -1748,11 +1796,11 @@
       <c r="AM14" s="9"/>
       <c r="AN14" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO14" s="9">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:44" x14ac:dyDescent="0.2">
@@ -1765,8 +1813,12 @@
       <c r="C15" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
+      <c r="D15" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
@@ -1803,7 +1855,7 @@
       <c r="AM15" s="9"/>
       <c r="AN15" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AO15" s="9">
         <f t="shared" si="2"/>
@@ -1820,8 +1872,12 @@
       <c r="C16" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
+      <c r="D16" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
@@ -1858,7 +1914,7 @@
       <c r="AM16" s="9"/>
       <c r="AN16" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AO16" s="9">
         <f t="shared" si="2"/>
@@ -1875,8 +1931,12 @@
       <c r="C17" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
+      <c r="D17" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
@@ -1913,11 +1973,11 @@
       <c r="AM17" s="9"/>
       <c r="AN17" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO17" s="9">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:41" x14ac:dyDescent="0.2">
@@ -1930,8 +1990,12 @@
       <c r="C18" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
+      <c r="D18" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
@@ -1968,7 +2032,7 @@
       <c r="AM18" s="9"/>
       <c r="AN18" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AO18" s="9">
         <f t="shared" si="2"/>
@@ -1985,8 +2049,12 @@
       <c r="C19" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
+      <c r="D19" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>10</v>
+      </c>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
       <c r="H19" s="9"/>
@@ -2023,11 +2091,11 @@
       <c r="AM19" s="9"/>
       <c r="AN19" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO19" s="9">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:41" x14ac:dyDescent="0.2">
@@ -2040,8 +2108,12 @@
       <c r="C20" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
+      <c r="D20" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
       <c r="H20" s="9"/>
@@ -2078,11 +2150,11 @@
       <c r="AM20" s="9"/>
       <c r="AN20" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO20" s="9">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:41" x14ac:dyDescent="0.2">
@@ -2095,8 +2167,12 @@
       <c r="C21" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
+      <c r="D21" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>10</v>
+      </c>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
@@ -2137,7 +2213,7 @@
       </c>
       <c r="AO21" s="9">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:41" x14ac:dyDescent="0.2">
@@ -2150,8 +2226,12 @@
       <c r="C22" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
+      <c r="D22" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
       <c r="H22" s="9"/>
@@ -2188,7 +2268,7 @@
       <c r="AM22" s="9"/>
       <c r="AN22" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AO22" s="9">
         <f t="shared" si="2"/>
@@ -2205,8 +2285,12 @@
       <c r="C23" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
+      <c r="D23" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
       <c r="H23" s="9"/>
@@ -2243,7 +2327,7 @@
       <c r="AM23" s="9"/>
       <c r="AN23" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AO23" s="9">
         <f t="shared" si="2"/>
@@ -2260,8 +2344,12 @@
       <c r="C24" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
+      <c r="D24" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
       <c r="H24" s="9"/>
@@ -2298,7 +2386,7 @@
       <c r="AM24" s="9"/>
       <c r="AN24" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AO24" s="9">
         <f t="shared" si="2"/>
@@ -2315,8 +2403,12 @@
       <c r="C25" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
+      <c r="D25" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>10</v>
+      </c>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
       <c r="H25" s="9"/>
@@ -2353,11 +2445,11 @@
       <c r="AM25" s="9"/>
       <c r="AN25" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO25" s="9">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:41" x14ac:dyDescent="0.2">
@@ -2370,8 +2462,12 @@
       <c r="C26" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
+      <c r="D26" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
       <c r="H26" s="9"/>
@@ -2408,7 +2504,7 @@
       <c r="AM26" s="9"/>
       <c r="AN26" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AO26" s="9">
         <f t="shared" si="2"/>
@@ -2425,8 +2521,12 @@
       <c r="C27" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
+      <c r="D27" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
@@ -2463,7 +2563,7 @@
       <c r="AM27" s="9"/>
       <c r="AN27" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AO27" s="9">
         <f t="shared" si="2"/>
@@ -2480,8 +2580,12 @@
       <c r="C28" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
+      <c r="D28" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
       <c r="H28" s="9"/>
@@ -2518,7 +2622,7 @@
       <c r="AM28" s="9"/>
       <c r="AN28" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AO28" s="9">
         <f t="shared" si="2"/>
@@ -2535,8 +2639,12 @@
       <c r="C29" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
+      <c r="D29" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>10</v>
+      </c>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
@@ -2573,11 +2681,11 @@
       <c r="AM29" s="9"/>
       <c r="AN29" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO29" s="9">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:41" x14ac:dyDescent="0.2">
@@ -2590,8 +2698,12 @@
       <c r="C30" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
+      <c r="D30" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
       <c r="H30" s="9"/>
@@ -2628,7 +2740,7 @@
       <c r="AM30" s="9"/>
       <c r="AN30" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AO30" s="9">
         <f t="shared" si="2"/>
@@ -2645,8 +2757,12 @@
       <c r="C31" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
+      <c r="D31" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
       <c r="H31" s="9"/>
@@ -2683,7 +2799,7 @@
       <c r="AM31" s="9"/>
       <c r="AN31" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AO31" s="9">
         <f t="shared" si="2"/>
@@ -2700,8 +2816,12 @@
       <c r="C32" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
+      <c r="D32" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="F32" s="9"/>
       <c r="G32" s="9"/>
       <c r="H32" s="9"/>
@@ -2738,7 +2858,7 @@
       <c r="AM32" s="9"/>
       <c r="AN32" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AO32" s="9">
         <f t="shared" si="2"/>
@@ -2755,8 +2875,12 @@
       <c r="C33" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
+      <c r="D33" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="F33" s="9"/>
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
@@ -2793,7 +2917,7 @@
       <c r="AM33" s="9"/>
       <c r="AN33" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AO33" s="9">
         <f t="shared" si="2"/>
@@ -2810,8 +2934,12 @@
       <c r="C34" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
+      <c r="D34" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="F34" s="9"/>
       <c r="G34" s="9"/>
       <c r="H34" s="9"/>
@@ -2848,11 +2976,11 @@
       <c r="AM34" s="9"/>
       <c r="AN34" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO34" s="9">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:41" x14ac:dyDescent="0.2">
@@ -2865,8 +2993,12 @@
       <c r="C35" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
+      <c r="D35" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="F35" s="9"/>
       <c r="G35" s="9"/>
       <c r="H35" s="9"/>
@@ -2903,7 +3035,7 @@
       <c r="AM35" s="9"/>
       <c r="AN35" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AO35" s="9">
         <f t="shared" si="2"/>
@@ -2920,8 +3052,12 @@
       <c r="C36" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
+      <c r="D36" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="F36" s="9"/>
       <c r="G36" s="9"/>
       <c r="H36" s="9"/>
@@ -2958,11 +3094,11 @@
       <c r="AM36" s="9"/>
       <c r="AN36" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO36" s="9">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:41" x14ac:dyDescent="0.2">
@@ -2975,8 +3111,12 @@
       <c r="C37" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D37" s="9"/>
-      <c r="E37" s="9"/>
+      <c r="D37" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="F37" s="9"/>
       <c r="G37" s="9"/>
       <c r="H37" s="9"/>
@@ -3013,11 +3153,11 @@
       <c r="AM37" s="9"/>
       <c r="AN37" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO37" s="9">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:41" x14ac:dyDescent="0.2">
@@ -3030,8 +3170,12 @@
       <c r="C38" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
+      <c r="D38" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="F38" s="9"/>
       <c r="G38" s="9"/>
       <c r="H38" s="9"/>
@@ -3068,7 +3212,7 @@
       <c r="AM38" s="9"/>
       <c r="AN38" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AO38" s="9">
         <f t="shared" si="2"/>
@@ -3085,8 +3229,12 @@
       <c r="C39" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
+      <c r="D39" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="F39" s="9"/>
       <c r="G39" s="9"/>
       <c r="H39" s="9"/>
@@ -3123,7 +3271,7 @@
       <c r="AM39" s="9"/>
       <c r="AN39" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AO39" s="9">
         <f t="shared" si="2"/>
@@ -3140,8 +3288,12 @@
       <c r="C40" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D40" s="9"/>
-      <c r="E40" s="9"/>
+      <c r="D40" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="F40" s="9"/>
       <c r="G40" s="9"/>
       <c r="H40" s="9"/>
@@ -3178,7 +3330,7 @@
       <c r="AM40" s="9"/>
       <c r="AN40" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AO40" s="9">
         <f t="shared" si="2"/>
@@ -3195,8 +3347,12 @@
       <c r="C41" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D41" s="9"/>
-      <c r="E41" s="9"/>
+      <c r="D41" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="F41" s="9"/>
       <c r="G41" s="9"/>
       <c r="H41" s="9"/>
@@ -3233,7 +3389,7 @@
       <c r="AM41" s="9"/>
       <c r="AN41" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AO41" s="9">
         <f t="shared" si="2"/>
@@ -3250,8 +3406,12 @@
       <c r="C42" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D42" s="9"/>
-      <c r="E42" s="9"/>
+      <c r="D42" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="F42" s="9"/>
       <c r="G42" s="9"/>
       <c r="H42" s="9"/>
@@ -3288,7 +3448,7 @@
       <c r="AM42" s="9"/>
       <c r="AN42" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AO42" s="9">
         <f t="shared" si="2"/>
@@ -3305,8 +3465,12 @@
       <c r="C43" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D43" s="9"/>
-      <c r="E43" s="9"/>
+      <c r="D43" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="F43" s="9"/>
       <c r="G43" s="9"/>
       <c r="H43" s="9"/>
@@ -3343,7 +3507,7 @@
       <c r="AM43" s="9"/>
       <c r="AN43" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AO43" s="9">
         <f t="shared" si="2"/>
@@ -3360,8 +3524,12 @@
       <c r="C44" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D44" s="9"/>
-      <c r="E44" s="9"/>
+      <c r="D44" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E44" s="9" t="s">
+        <v>10</v>
+      </c>
       <c r="F44" s="9"/>
       <c r="G44" s="9"/>
       <c r="H44" s="9"/>
@@ -3398,11 +3566,11 @@
       <c r="AM44" s="9"/>
       <c r="AN44" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO44" s="9">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:41" x14ac:dyDescent="0.2">
@@ -3415,8 +3583,12 @@
       <c r="C45" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D45" s="9"/>
-      <c r="E45" s="9"/>
+      <c r="D45" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="F45" s="9"/>
       <c r="G45" s="9"/>
       <c r="H45" s="9"/>
@@ -3453,7 +3625,7 @@
       <c r="AM45" s="9"/>
       <c r="AN45" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AO45" s="9">
         <f t="shared" si="2"/>
@@ -3470,8 +3642,12 @@
       <c r="C46" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D46" s="9"/>
-      <c r="E46" s="9"/>
+      <c r="D46" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E46" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="F46" s="9"/>
       <c r="G46" s="9"/>
       <c r="H46" s="9"/>
@@ -3508,7 +3684,7 @@
       <c r="AM46" s="9"/>
       <c r="AN46" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AO46" s="9">
         <f t="shared" si="2"/>
@@ -3525,8 +3701,12 @@
       <c r="C47" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="D47" s="9"/>
-      <c r="E47" s="9"/>
+      <c r="D47" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E47" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="F47" s="9"/>
       <c r="G47" s="9"/>
       <c r="H47" s="9"/>
@@ -3563,11 +3743,11 @@
       <c r="AM47" s="9"/>
       <c r="AN47" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO47" s="9">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:41" x14ac:dyDescent="0.2">
@@ -3580,8 +3760,12 @@
       <c r="C48" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="D48" s="9"/>
-      <c r="E48" s="9"/>
+      <c r="D48" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E48" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="F48" s="9"/>
       <c r="G48" s="9"/>
       <c r="H48" s="9"/>
@@ -3618,7 +3802,7 @@
       <c r="AM48" s="9"/>
       <c r="AN48" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AO48" s="9">
         <f t="shared" si="2"/>
@@ -3635,8 +3819,12 @@
       <c r="C49" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="D49" s="9"/>
-      <c r="E49" s="9"/>
+      <c r="D49" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E49" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="F49" s="9"/>
       <c r="G49" s="9"/>
       <c r="H49" s="9"/>
@@ -3673,7 +3861,7 @@
       <c r="AM49" s="9"/>
       <c r="AN49" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AO49" s="9">
         <f t="shared" si="2"/>
@@ -3690,8 +3878,12 @@
       <c r="C50" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D50" s="9"/>
-      <c r="E50" s="9"/>
+      <c r="D50" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E50" s="9" t="s">
+        <v>10</v>
+      </c>
       <c r="F50" s="9"/>
       <c r="G50" s="9"/>
       <c r="H50" s="9"/>
@@ -3732,7 +3924,7 @@
       </c>
       <c r="AO50" s="9">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51" spans="1:41" x14ac:dyDescent="0.2">
@@ -3745,8 +3937,12 @@
       <c r="C51" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D51" s="9"/>
-      <c r="E51" s="9"/>
+      <c r="D51" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E51" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="F51" s="9"/>
       <c r="G51" s="9"/>
       <c r="H51" s="9"/>
@@ -3783,7 +3979,7 @@
       <c r="AM51" s="9"/>
       <c r="AN51" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AO51" s="9">
         <f t="shared" si="2"/>
@@ -3800,8 +3996,12 @@
       <c r="C52" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D52" s="9"/>
-      <c r="E52" s="9"/>
+      <c r="D52" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E52" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="F52" s="9"/>
       <c r="G52" s="9"/>
       <c r="H52" s="9"/>
@@ -3838,7 +4038,7 @@
       <c r="AM52" s="9"/>
       <c r="AN52" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AO52" s="9">
         <f t="shared" si="2"/>

</xml_diff>